<commit_message>
Regerated outputs for ACR with regards to a change in inv.dh-relper.01 to "At least one related person identifier shall at least have a system and a value"
CIFMM-2735
</commit_message>
<xml_diff>
--- a/output/AdvanceCareRecords/practitioner-ident-1.xlsx
+++ b/output/AdvanceCareRecords/practitioner-ident-1.xlsx
@@ -156,7 +156,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}inv-dh-prac-01:The practitioner shall at least have one identifier with a system and a value {identifier.where(system.count() + value.count() &gt;1).exists()}</t>
+dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}inv-dh-prac-01:At least one practitioner identifier shall at least have a system and a value {identifier.where(system.count() + value.count() &gt;1).exists()}</t>
   </si>
   <si>
     <t>PRD (as one example)</t>
@@ -997,7 +997,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-inv-dh-prac-02:The issuer reference shall at least have a reference, an identifier or a display {issuer.exists() implies issuer.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}inv-dh-prac-03:The issuer organisation shall conform to Base Organization {issuer.reference.exists() implies issuer.all($this.reference.resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/organization-dh-base-1'))}</t>
+inv-dh-prac-02:If present, an issuer shall at least have a reference, an identifier or a display {issuer.exists() implies issuer.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}inv-dh-prac-03:If present, an issuer organisation shall conform to Base Organization {issuer.reference.exists() implies issuer.all($this.reference.resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/organization-dh-base-1'))}</t>
   </si>
   <si>
     <t>CER?</t>

</xml_diff>